<commit_message>
Fix network proxy problem.
</commit_message>
<xml_diff>
--- a/excel/en/MCP SOFR Curve (BBG).xlsx
+++ b/excel/en/MCP SOFR Curve (BBG).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\vuepress\help-master3\latest\api\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{657C8DF4-9E66-4446-9611-7CE5E414F9B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38ED47A8-79FD-4284-8FB8-D2BDE3B75B5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="22920" windowHeight="13890" tabRatio="904" activeTab="3" xr2:uid="{4CD82504-096D-4517-A904-95A625040DFB}"/>
   </bookViews>
@@ -1347,9 +1347,6 @@
     <t>OIS swap Data Set</t>
   </si>
   <si>
-    <t>Curver Data Set</t>
-  </si>
-  <si>
     <t>Swap Curve Object</t>
   </si>
   <si>
@@ -1366,6 +1363,9 @@
   </si>
   <si>
     <t>Fwd Rate</t>
+  </si>
+  <si>
+    <t>Curve Data Set</t>
   </si>
 </sst>
 </file>
@@ -1993,10 +1993,10 @@
                   <c:v>4.2470777446765626E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>4.1970591523764721E-2</c:v>
+                  <c:v>4.1970591523764728E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>4.1358346381758532E-2</c:v>
+                  <c:v>4.1358346381758525E-2</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>4.0716373841928243E-2</c:v>
@@ -2005,25 +2005,25 @@
                   <c:v>4.0162889053504743E-2</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>3.960254039413777E-2</c:v>
+                  <c:v>3.9602540394137763E-2</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>3.9044902274860772E-2</c:v>
+                  <c:v>3.9044902274861029E-2</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>3.8609017706586007E-2</c:v>
+                  <c:v>3.8609017706585792E-2</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>3.8137719875804228E-2</c:v>
+                  <c:v>3.813771987580445E-2</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>3.5981909462809436E-2</c:v>
+                  <c:v>3.598190946280886E-2</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>3.4885479235119067E-2</c:v>
+                  <c:v>3.4885479235118616E-2</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>3.4420118019967708E-2</c:v>
+                  <c:v>3.4420118019967E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2193,22 +2193,22 @@
                   <c:v>0.97039261596048143</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.96758937684214719</c:v>
+                  <c:v>0.96758937684214696</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.96508272887245383</c:v>
+                  <c:v>0.96508272887245405</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.96237923224640232</c:v>
+                  <c:v>0.96237923224640209</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.94722434261729571</c:v>
+                  <c:v>0.94722434261729649</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.93242914731632554</c:v>
+                  <c:v>0.93242914731632631</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.90157847733597318</c:v>
+                  <c:v>0.90157847733597507</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -12837,8 +12837,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{009CD23B-43E6-4D6C-A20A-16925A5C8840}">
   <dimension ref="B1:Q119"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B91" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="I106" sqref="I106:I113"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -13011,7 +13011,7 @@
     </row>
     <row r="15" spans="2:15" ht="16.5" thickTop="1" thickBot="1">
       <c r="B15" s="3" t="s">
-        <v>363</v>
+        <v>369</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>11</v>
@@ -13025,7 +13025,7 @@
     </row>
     <row r="16" spans="2:15" ht="16.5" thickTop="1" thickBot="1">
       <c r="B16" s="3" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>12</v>
@@ -13113,10 +13113,10 @@
     </row>
     <row r="22" spans="2:17" ht="15.75" thickTop="1">
       <c r="D22" t="s">
+        <v>364</v>
+      </c>
+      <c r="E22" t="s">
         <v>365</v>
-      </c>
-      <c r="E22" t="s">
-        <v>366</v>
       </c>
       <c r="G22" t="s">
         <v>337</v>
@@ -13770,10 +13770,10 @@
     </row>
     <row r="58" spans="2:10" ht="15.75" thickTop="1">
       <c r="D58" t="s">
+        <v>364</v>
+      </c>
+      <c r="E58" t="s">
         <v>365</v>
-      </c>
-      <c r="E58" t="s">
-        <v>366</v>
       </c>
       <c r="G58" s="1"/>
     </row>
@@ -14056,7 +14056,7 @@
       </c>
       <c r="E70" s="26">
         <f>_xll.SwapCurveZeroRate($D$16,C70)</f>
-        <v>4.1970591523764721E-2</v>
+        <v>4.1970591523764728E-2</v>
       </c>
       <c r="G70">
         <v>0.98233499999999996</v>
@@ -14070,7 +14070,7 @@
       </c>
       <c r="J70">
         <f t="shared" si="1"/>
-        <v>-1.0915237647157738E-4</v>
+        <v>-1.0915237647246556E-4</v>
       </c>
     </row>
     <row r="71" spans="2:10" ht="16.5" thickTop="1" thickBot="1">
@@ -14087,7 +14087,7 @@
       </c>
       <c r="E71" s="26">
         <f>_xll.SwapCurveZeroRate($D$16,C71)</f>
-        <v>4.1358346381758532E-2</v>
+        <v>4.1358346381758525E-2</v>
       </c>
       <c r="G71">
         <v>0.97925600000000002</v>
@@ -14101,7 +14101,7 @@
       </c>
       <c r="J71">
         <f t="shared" si="1"/>
-        <v>-1.5463817585370521E-4</v>
+        <v>-1.5463817585281703E-4</v>
       </c>
     </row>
     <row r="72" spans="2:10" ht="16.5" thickTop="1" thickBot="1">
@@ -14180,7 +14180,7 @@
       </c>
       <c r="E74" s="26">
         <f>_xll.SwapCurveZeroRate($D$16,C74)</f>
-        <v>3.960254039413777E-2</v>
+        <v>3.9602540394137763E-2</v>
       </c>
       <c r="G74">
         <v>0.97039399999999998</v>
@@ -14194,7 +14194,7 @@
       </c>
       <c r="J74">
         <f t="shared" si="1"/>
-        <v>-2.2403941377691083E-4</v>
+        <v>-2.2403941377602266E-4</v>
       </c>
     </row>
     <row r="75" spans="2:10" ht="16.5" thickTop="1" thickBot="1">
@@ -14207,11 +14207,11 @@
       </c>
       <c r="D75" s="27">
         <f>_xll.SwapCurveDiscountFactor($D$16,C75)</f>
-        <v>0.96758937684214719</v>
+        <v>0.96758937684214696</v>
       </c>
       <c r="E75" s="26">
         <f>_xll.SwapCurveZeroRate($D$16,C75)</f>
-        <v>3.9044902274860772E-2</v>
+        <v>3.9044902274861029E-2</v>
       </c>
       <c r="G75">
         <v>0.96759099999999998</v>
@@ -14221,11 +14221,11 @@
       </c>
       <c r="I75" s="28">
         <f t="shared" si="0"/>
-        <v>1.623157852792545E-6</v>
+        <v>1.6231578530145896E-6</v>
       </c>
       <c r="J75">
         <f t="shared" si="1"/>
-        <v>-2.3022748607726129E-4</v>
+        <v>-2.3022748610301846E-4</v>
       </c>
     </row>
     <row r="76" spans="2:10" ht="16.5" thickTop="1" thickBot="1">
@@ -14238,11 +14238,11 @@
       </c>
       <c r="D76" s="27">
         <f>_xll.SwapCurveDiscountFactor($D$16,C76)</f>
-        <v>0.96508272887245383</v>
+        <v>0.96508272887245405</v>
       </c>
       <c r="E76" s="26">
         <f>_xll.SwapCurveZeroRate($D$16,C76)</f>
-        <v>3.8609017706586007E-2</v>
+        <v>3.8609017706585792E-2</v>
       </c>
       <c r="G76">
         <v>0.96508499999999997</v>
@@ -14252,11 +14252,11 @@
       </c>
       <c r="I76" s="28">
         <f t="shared" si="0"/>
-        <v>2.2711275461384517E-6</v>
+        <v>2.2711275459164071E-6</v>
       </c>
       <c r="J76">
         <f t="shared" si="1"/>
-        <v>-2.4177065860042646E-4</v>
+        <v>-2.4177065857911018E-4</v>
       </c>
     </row>
     <row r="77" spans="2:10" ht="16.5" thickTop="1" thickBot="1">
@@ -14269,11 +14269,11 @@
       </c>
       <c r="D77" s="27">
         <f>_xll.SwapCurveDiscountFactor($D$16,C77)</f>
-        <v>0.96237923224640232</v>
+        <v>0.96237923224640209</v>
       </c>
       <c r="E77" s="26">
         <f>_xll.SwapCurveZeroRate($D$16,C77)</f>
-        <v>3.8137719875804228E-2</v>
+        <v>3.813771987580445E-2</v>
       </c>
       <c r="G77">
         <v>0.96238199999999996</v>
@@ -14283,11 +14283,11 @@
       </c>
       <c r="I77" s="28">
         <f t="shared" si="0"/>
-        <v>2.7677535976433632E-6</v>
+        <v>2.7677535978654078E-6</v>
       </c>
       <c r="J77">
         <f t="shared" si="1"/>
-        <v>-2.4198758042270896E-4</v>
+        <v>-2.4198758044491342E-4</v>
       </c>
     </row>
     <row r="78" spans="2:10" ht="16.5" thickTop="1" thickBot="1">
@@ -14300,11 +14300,11 @@
       </c>
       <c r="D78" s="27">
         <f>_xll.SwapCurveDiscountFactor($D$16,C78)</f>
-        <v>0.94722434261729571</v>
+        <v>0.94722434261729649</v>
       </c>
       <c r="E78" s="26">
         <f>_xll.SwapCurveZeroRate($D$16,C78)</f>
-        <v>3.5981909462809436E-2</v>
+        <v>3.598190946280886E-2</v>
       </c>
       <c r="G78">
         <v>0.94719600000000004</v>
@@ -14314,11 +14314,11 @@
       </c>
       <c r="I78" s="28">
         <f t="shared" si="0"/>
-        <v>-2.8342617295673556E-5</v>
+        <v>-2.8342617296450712E-5</v>
       </c>
       <c r="J78">
         <f t="shared" si="1"/>
-        <v>1.9990537190563984E-3</v>
+        <v>1.99905371911413E-3</v>
       </c>
     </row>
     <row r="79" spans="2:10" ht="16.5" thickTop="1" thickBot="1">
@@ -14331,11 +14331,11 @@
       </c>
       <c r="D79" s="27">
         <f>_xll.SwapCurveDiscountFactor($D$16,C79)</f>
-        <v>0.93242914731632554</v>
+        <v>0.93242914731632631</v>
       </c>
       <c r="E79" s="26">
         <f>_xll.SwapCurveZeroRate($D$16,C79)</f>
-        <v>3.4885479235119067E-2</v>
+        <v>3.4885479235118616E-2</v>
       </c>
       <c r="G79">
         <v>0.93243399999999999</v>
@@ -14345,11 +14345,11 @@
       </c>
       <c r="I79" s="28">
         <f t="shared" si="0"/>
-        <v>4.8526836744500201E-6</v>
+        <v>4.852683673672864E-6</v>
       </c>
       <c r="J79">
         <f t="shared" si="1"/>
-        <v>-2.5792351190645491E-4</v>
+        <v>-2.579235118616019E-4</v>
       </c>
     </row>
     <row r="80" spans="2:10" ht="16.5" thickTop="1" thickBot="1">
@@ -14362,11 +14362,11 @@
       </c>
       <c r="D80" s="27">
         <f>_xll.SwapCurveDiscountFactor($D$16,C80)</f>
-        <v>0.90157847733597318</v>
+        <v>0.90157847733597507</v>
       </c>
       <c r="E80" s="26">
         <f>_xll.SwapCurveZeroRate($D$16,C80)</f>
-        <v>3.4420118019967708E-2</v>
+        <v>3.4420118019967E-2</v>
       </c>
       <c r="G80">
         <v>0.901586</v>
@@ -14376,11 +14376,11 @@
       </c>
       <c r="I80" s="28">
         <f t="shared" si="0"/>
-        <v>7.522664026815562E-6</v>
+        <v>7.5226640249281829E-6</v>
       </c>
       <c r="J80">
         <f t="shared" si="1"/>
-        <v>-1.2418019967705973E-3</v>
+        <v>-1.2418019966999871E-3</v>
       </c>
     </row>
     <row r="81" spans="2:10" ht="16.5" thickTop="1" thickBot="1">
@@ -14393,11 +14393,11 @@
       </c>
       <c r="D81" s="27">
         <f>_xll.SwapCurveDiscountFactor($D$16,C81)</f>
-        <v>0.86990993035393227</v>
+        <v>0.8699099303539346</v>
       </c>
       <c r="E81" s="26">
         <f>_xll.SwapCurveZeroRate($D$16,C81)</f>
-        <v>3.4793737601188923E-2</v>
+        <v>3.4793737601188243E-2</v>
       </c>
       <c r="G81">
         <v>0.86992000000000003</v>
@@ -14407,11 +14407,11 @@
       </c>
       <c r="I81" s="28">
         <f t="shared" si="0"/>
-        <v>1.0069646067756288E-5</v>
+        <v>1.006964606542482E-5</v>
       </c>
       <c r="J81">
         <f t="shared" si="1"/>
-        <v>-2.6637601188919113E-3</v>
+        <v>-2.6637601188239657E-3</v>
       </c>
     </row>
     <row r="82" spans="2:10" ht="16.5" thickTop="1" thickBot="1">
@@ -14424,11 +14424,11 @@
       </c>
       <c r="D82" s="27">
         <f>_xll.SwapCurveDiscountFactor($D$16,C82)</f>
-        <v>0.83761615479340845</v>
+        <v>0.83761615479340923</v>
       </c>
       <c r="E82" s="26">
         <f>_xll.SwapCurveZeroRate($D$16,C82)</f>
-        <v>3.5400271703527809E-2</v>
+        <v>3.5400271703527601E-2</v>
       </c>
       <c r="G82">
         <v>0.83762899999999996</v>
@@ -14438,11 +14438,11 @@
       </c>
       <c r="I82" s="28">
         <f t="shared" si="0"/>
-        <v>1.2845206591505232E-5</v>
+        <v>1.2845206590728075E-5</v>
       </c>
       <c r="J82">
         <f t="shared" si="1"/>
-        <v>-2.2471703527808806E-3</v>
+        <v>-2.2471703527600084E-3</v>
       </c>
     </row>
     <row r="83" spans="2:10" ht="16.5" thickTop="1" thickBot="1">
@@ -14455,11 +14455,11 @@
       </c>
       <c r="D83" s="27">
         <f>_xll.SwapCurveDiscountFactor($D$16,C83)</f>
-        <v>0.80517676814690109</v>
+        <v>0.80517676814690176</v>
       </c>
       <c r="E83" s="26">
         <f>_xll.SwapCurveZeroRate($D$16,C83)</f>
-        <v>3.6082620819753046E-2</v>
+        <v>3.6082620819752907E-2</v>
       </c>
       <c r="G83">
         <v>0.80519300000000005</v>
@@ -14469,11 +14469,11 @@
       </c>
       <c r="I83" s="28">
         <f t="shared" si="0"/>
-        <v>1.6231853098958027E-5</v>
+        <v>1.6231853098291893E-5</v>
       </c>
       <c r="J83">
         <f t="shared" si="1"/>
-        <v>-1.9820819753046948E-3</v>
+        <v>-1.982081975290928E-3</v>
       </c>
     </row>
     <row r="84" spans="2:10" ht="16.5" thickTop="1" thickBot="1">
@@ -14486,11 +14486,11 @@
       </c>
       <c r="D84" s="27">
         <f>_xll.SwapCurveDiscountFactor($D$16,C84)</f>
-        <v>0.77297424927231739</v>
+        <v>0.77297424927231895</v>
       </c>
       <c r="E84" s="26">
         <f>_xll.SwapCurveZeroRate($D$16,C84)</f>
-        <v>3.6748369525088684E-2</v>
+        <v>3.6748369525088399E-2</v>
       </c>
       <c r="G84">
         <v>0.77299200000000001</v>
@@ -14500,11 +14500,11 @@
       </c>
       <c r="I84" s="28">
         <f t="shared" si="0"/>
-        <v>1.7750727682619427E-5</v>
+        <v>1.7750727681065115E-5</v>
       </c>
       <c r="J84">
         <f t="shared" si="1"/>
-        <v>-2.2169525088679976E-3</v>
+        <v>-2.2169525088395758E-3</v>
       </c>
     </row>
     <row r="85" spans="2:10" ht="16.5" thickTop="1" thickBot="1">
@@ -14517,11 +14517,11 @@
       </c>
       <c r="D85" s="27">
         <f>_xll.SwapCurveDiscountFactor($D$16,C85)</f>
-        <v>0.74141558603620994</v>
+        <v>0.74141558603620872</v>
       </c>
       <c r="E85" s="26">
         <f>_xll.SwapCurveZeroRate($D$16,C85)</f>
-        <v>3.7348083997045034E-2</v>
+        <v>3.7348083997045228E-2</v>
       </c>
       <c r="G85">
         <v>0.74143599999999998</v>
@@ -14531,11 +14531,11 @@
       </c>
       <c r="I85" s="28">
         <f t="shared" si="0"/>
-        <v>2.0413963790044676E-5</v>
+        <v>2.0413963791265921E-5</v>
       </c>
       <c r="J85">
         <f t="shared" si="1"/>
-        <v>-2.908399704503406E-3</v>
+        <v>-2.9083997045229459E-3</v>
       </c>
     </row>
     <row r="86" spans="2:10" ht="16.5" thickTop="1" thickBot="1">
@@ -14548,11 +14548,11 @@
       </c>
       <c r="D86" s="27">
         <f>_xll.SwapCurveDiscountFactor($D$16,C86)</f>
-        <v>0.71072249318149572</v>
+        <v>0.71072249318149794</v>
       </c>
       <c r="E86" s="26">
         <f>_xll.SwapCurveZeroRate($D$16,C86)</f>
-        <v>3.7906851905557863E-2</v>
+        <v>3.7906851905557502E-2</v>
       </c>
       <c r="G86">
         <v>0.71074599999999999</v>
@@ -14562,11 +14562,11 @@
       </c>
       <c r="I86" s="28">
         <f t="shared" si="0"/>
-        <v>2.3506818504270832E-5</v>
+        <v>2.3506818502050386E-5</v>
       </c>
       <c r="J86">
         <f t="shared" si="1"/>
-        <v>-2.6751905557862443E-3</v>
+        <v>-2.6751905557502731E-3</v>
       </c>
     </row>
     <row r="87" spans="2:10" ht="16.5" thickTop="1" thickBot="1">
@@ -14579,11 +14579,11 @@
       </c>
       <c r="D87" s="27">
         <f>_xll.SwapCurveDiscountFactor($D$16,C87)</f>
-        <v>0.68070235536113155</v>
+        <v>0.68070235536113133</v>
       </c>
       <c r="E87" s="26">
         <f>_xll.SwapCurveZeroRate($D$16,C87)</f>
-        <v>3.844194975092699E-2</v>
+        <v>3.8441949750927032E-2</v>
       </c>
       <c r="G87">
         <v>0.680728</v>
@@ -14593,11 +14593,11 @@
       </c>
       <c r="I87" s="28">
         <f t="shared" si="0"/>
-        <v>2.5644638868449476E-5</v>
+        <v>2.5644638868671521E-5</v>
       </c>
       <c r="J87">
         <f t="shared" si="1"/>
-        <v>-2.48497509269896E-3</v>
+        <v>-2.4849750927034009E-3</v>
       </c>
     </row>
     <row r="88" spans="2:10" ht="16.5" thickTop="1" thickBot="1">
@@ -14610,11 +14610,11 @@
       </c>
       <c r="D88" s="27">
         <f>_xll.SwapCurveDiscountFactor($D$16,C88)</f>
-        <v>0.62315129374496736</v>
+        <v>0.62315129374496692</v>
       </c>
       <c r="E88" s="26">
         <f>_xll.SwapCurveZeroRate($D$16,C88)</f>
-        <v>3.9395839580037909E-2</v>
+        <v>3.9395839580037964E-2</v>
       </c>
       <c r="G88">
         <v>0.62319199999999997</v>
@@ -14624,11 +14624,11 @@
       </c>
       <c r="I88" s="28">
         <f t="shared" si="0"/>
-        <v>4.0706255032607608E-5</v>
+        <v>4.0706255033051697E-5</v>
       </c>
       <c r="J88">
         <f t="shared" si="1"/>
-        <v>-3.2339580037907822E-3</v>
+        <v>-3.2339580037965554E-3</v>
       </c>
     </row>
     <row r="89" spans="2:10" ht="16.5" thickTop="1" thickBot="1">
@@ -14641,11 +14641,11 @@
       </c>
       <c r="D89" s="27">
         <f>_xll.SwapCurveDiscountFactor($D$16,C89)</f>
-        <v>0.54519068535052073</v>
+        <v>0.54519068535052118</v>
       </c>
       <c r="E89" s="26">
         <f>_xll.SwapCurveZeroRate($D$16,C89)</f>
-        <v>4.0421441630822029E-2</v>
+        <v>4.042144163082198E-2</v>
       </c>
       <c r="G89">
         <v>0.54526399999999997</v>
@@ -14655,11 +14655,11 @@
       </c>
       <c r="I89" s="28">
         <f t="shared" si="0"/>
-        <v>7.3314649479239158E-5</v>
+        <v>7.3314649478795069E-5</v>
       </c>
       <c r="J89">
         <f t="shared" si="1"/>
-        <v>-3.3341630822034674E-3</v>
+        <v>-3.3341630821981383E-3</v>
       </c>
     </row>
     <row r="90" spans="2:10" ht="16.5" thickTop="1" thickBot="1">
@@ -14672,11 +14672,11 @@
       </c>
       <c r="D90" s="27">
         <f>_xll.SwapCurveDiscountFactor($D$16,C90)</f>
-        <v>0.4397635964737307</v>
+        <v>0.43976359647373037</v>
       </c>
       <c r="E90" s="26">
         <f>_xll.SwapCurveZeroRate($D$16,C90)</f>
-        <v>4.1059025287882321E-2</v>
+        <v>4.1059025287882363E-2</v>
       </c>
       <c r="G90">
         <v>0.43987900000000002</v>
@@ -14686,11 +14686,11 @@
       </c>
       <c r="I90" s="28">
         <f t="shared" si="0"/>
-        <v>1.1540352626931982E-4</v>
+        <v>1.1540352626965289E-4</v>
       </c>
       <c r="J90">
         <f t="shared" si="1"/>
-        <v>-4.1225287882324935E-3</v>
+        <v>-4.1225287882369344E-3</v>
       </c>
     </row>
     <row r="91" spans="2:10" ht="16.5" thickTop="1" thickBot="1">
@@ -14703,11 +14703,11 @@
       </c>
       <c r="D91" s="27">
         <f>_xll.SwapCurveDiscountFactor($D$16,C91)</f>
-        <v>0.36318213455071108</v>
+        <v>0.36318213455070991</v>
       </c>
       <c r="E91" s="26">
         <f>_xll.SwapCurveZeroRate($D$16,C91)</f>
-        <v>4.0496281104630265E-2</v>
+        <v>4.0496281104630397E-2</v>
       </c>
       <c r="G91">
         <v>0.36325000000000002</v>
@@ -14717,11 +14717,11 @@
       </c>
       <c r="I91" s="28">
         <f t="shared" si="0"/>
-        <v>6.7865449288939672E-5</v>
+        <v>6.7865449290105406E-5</v>
       </c>
       <c r="J91">
         <f t="shared" si="1"/>
-        <v>-3.4081104630265813E-3</v>
+        <v>-3.4081104630399039E-3</v>
       </c>
     </row>
     <row r="92" spans="2:10" ht="16.5" thickTop="1" thickBot="1">
@@ -14734,11 +14734,11 @@
       </c>
       <c r="D92" s="27">
         <f>_xll.SwapCurveDiscountFactor($D$16,C92)</f>
-        <v>0.30621756033856617</v>
+        <v>0.30621756033856601</v>
       </c>
       <c r="E92" s="26">
         <f>_xll.SwapCurveZeroRate($D$16,C92)</f>
-        <v>3.9441444355182272E-2</v>
+        <v>3.9441444355182292E-2</v>
       </c>
       <c r="G92">
         <v>0.306228</v>
@@ -14748,11 +14748,11 @@
       </c>
       <c r="I92" s="28">
         <f t="shared" si="0"/>
-        <v>1.0439661433825353E-5</v>
+        <v>1.0439661433991887E-5</v>
       </c>
       <c r="J92">
         <f t="shared" si="1"/>
-        <v>-2.6344355182272849E-3</v>
+        <v>-2.6344355182290613E-3</v>
       </c>
     </row>
     <row r="93" spans="2:10" ht="16.5" thickTop="1" thickBot="1">
@@ -14765,11 +14765,11 @@
       </c>
       <c r="D93" s="27">
         <f>_xll.SwapCurveDiscountFactor($D$16,C93)</f>
-        <v>0.23218270147565548</v>
+        <v>0.23218270147565492</v>
       </c>
       <c r="E93" s="26">
         <f>_xll.SwapCurveZeroRate($D$16,C93)</f>
-        <v>3.6500767666732131E-2</v>
+        <v>3.6500767666732194E-2</v>
       </c>
       <c r="G93">
         <v>0.23179</v>
@@ -14779,11 +14779,11 @@
       </c>
       <c r="I93" s="28">
         <f t="shared" si="0"/>
-        <v>-3.9270147565548252E-4</v>
+        <v>-3.9270147565492741E-4</v>
       </c>
       <c r="J93">
         <f t="shared" si="1"/>
-        <v>1.7232333267869215E-3</v>
+        <v>1.7232333267807043E-3</v>
       </c>
     </row>
     <row r="94" spans="2:10" ht="16.5" thickTop="1" thickBot="1">
@@ -14796,11 +14796,11 @@
       </c>
       <c r="D94" s="27">
         <f>_xll.SwapCurveDiscountFactor($D$16,C94)</f>
-        <v>0.1881707398167711</v>
+        <v>0.1881707398167714</v>
       </c>
       <c r="E94" s="26">
         <f>_xll.SwapCurveZeroRate($D$16,C94)</f>
-        <v>3.3404449994215372E-2</v>
+        <v>3.3404449994215338E-2</v>
       </c>
       <c r="G94">
         <v>0.18759000000000001</v>
@@ -14810,11 +14810,11 @@
       </c>
       <c r="I94" s="28">
         <f t="shared" si="0"/>
-        <v>-5.8073981677109199E-4</v>
+        <v>-5.807398167713973E-4</v>
       </c>
       <c r="J94">
         <f t="shared" si="1"/>
-        <v>3.975000578462673E-3</v>
+        <v>3.9750005784662257E-3</v>
       </c>
     </row>
     <row r="95" spans="2:10" ht="15.75" thickTop="1"/>
@@ -14824,11 +14824,11 @@
       </c>
       <c r="I96" s="28">
         <f>AVERAGE(I63:I94)</f>
-        <v>-1.7189694828576539E-5</v>
+        <v>-1.7189694828808125E-5</v>
       </c>
       <c r="J96" s="28">
         <f>AVERAGE(J63:J94)</f>
-        <v>-5.1352642379244584E-4</v>
+        <v>-5.1352642378407753E-4</v>
       </c>
     </row>
     <row r="102" spans="2:11" ht="15.75" thickBot="1">
@@ -14862,31 +14862,31 @@
     </row>
     <row r="105" spans="2:11">
       <c r="C105" t="s">
+        <v>366</v>
+      </c>
+      <c r="D105" t="s">
         <v>367</v>
       </c>
-      <c r="D105" t="s">
+      <c r="E105" t="s">
         <v>368</v>
       </c>
-      <c r="E105" t="s">
-        <v>369</v>
-      </c>
       <c r="F105" t="s">
+        <v>366</v>
+      </c>
+      <c r="G105" t="s">
         <v>367</v>
       </c>
-      <c r="G105" t="s">
+      <c r="H105" t="s">
         <v>368</v>
       </c>
-      <c r="H105" t="s">
-        <v>369</v>
-      </c>
       <c r="I105" t="s">
+        <v>366</v>
+      </c>
+      <c r="J105" t="s">
         <v>367</v>
       </c>
-      <c r="J105" t="s">
+      <c r="K105" t="s">
         <v>368</v>
-      </c>
-      <c r="K105" t="s">
-        <v>369</v>
       </c>
     </row>
     <row r="106" spans="2:11">
@@ -15091,7 +15091,7 @@
       </c>
       <c r="K110" s="16">
         <f>_xll.YieldCurveForwardRate($D$16,I110,J110)</f>
-        <v>3.6987062023380042E-2</v>
+        <v>3.6987062023380486E-2</v>
       </c>
     </row>
     <row r="111" spans="2:11">
@@ -15132,7 +15132,7 @@
       </c>
       <c r="K111" s="16">
         <f>_xll.YieldCurveForwardRate($D$16,I111,J111)</f>
-        <v>3.6048740440704705E-2</v>
+        <v>3.6048740440704261E-2</v>
       </c>
     </row>
     <row r="112" spans="2:11">
@@ -15173,7 +15173,7 @@
       </c>
       <c r="K112" s="16">
         <f>_xll.YieldCurveForwardRate($D$16,I112,J112)</f>
-        <v>3.5168812028629877E-2</v>
+        <v>3.5168812028630321E-2</v>
       </c>
     </row>
     <row r="113" spans="2:11">
@@ -15190,7 +15190,7 @@
       </c>
       <c r="E113" s="16">
         <f>_xll.YieldCurveForwardRate($D$16,C113,D113)</f>
-        <v>3.3476123540173437E-2</v>
+        <v>3.3476123540170981E-2</v>
       </c>
       <c r="F113" s="1">
         <f>_xll.CalendarValueDateTenor($H$17,$D$3,$B113)</f>
@@ -15202,7 +15202,7 @@
       </c>
       <c r="H113" s="16">
         <f>_xll.YieldCurveForwardRate($D$16,F113,G113)</f>
-        <v>3.2876308198552806E-2</v>
+        <v>3.2876308198551023E-2</v>
       </c>
       <c r="I113" s="1">
         <f>_xll.CalendarValueDateTenor($H$17,$D$3,$B113)</f>
@@ -15214,7 +15214,7 @@
       </c>
       <c r="K113" s="16">
         <f>_xll.YieldCurveForwardRate($D$16,I113,J113)</f>
-        <v>3.1911094651729158E-2</v>
+        <v>3.1911094651726944E-2</v>
       </c>
     </row>
     <row r="119" spans="2:11" s="23" customFormat="1"/>
@@ -15755,7 +15755,7 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D86B0371-78B8-4F05-9D95-F21D4B0EBAC0}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{73F244A5-B3A2-4CC0-94B1-EC93F073A6B0}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="urn:pyxll:metadata"/>
   </ds:schemaRefs>

</xml_diff>